<commit_message>
changes - Se modifico el excel y se cambio titulo de un ejercicio
</commit_message>
<xml_diff>
--- a/Practicas/notas/Notas.xlsx
+++ b/Practicas/notas/Notas.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evomatik/proyectos/ProyectoJavascript/JavascriptProjectV-1.0/Practicas/notas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlanLeidyCarlos\Desktop\JavascriptProject\JavascriptProjectV-1.0\Practicas\notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95458587-AF4A-4CDE-9BC0-D6B8F0BE60D9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16425" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicios con javascript_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicios de javascript_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Num</t>
   </si>
@@ -39,13 +41,58 @@
   </si>
   <si>
     <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Escribir un texto en un input y mostra lo en un alert de bootstrap</t>
+  </si>
+  <si>
+    <t>Escribir el nombre y la edad de una persona y mostrar los datos asi como decir si es mayor o menor de edad</t>
+  </si>
+  <si>
+    <t>Covertir de pesos a dolares con el valor actual del dólar</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>Sacar el area de un Rectangulo</t>
+  </si>
+  <si>
+    <t>Sacar el perimetro de un Cuadrado</t>
+  </si>
+  <si>
+    <t>Sacar el volumen de un Esfera</t>
+  </si>
+  <si>
+    <t>Leer un valor y determinar si es mayor a 100</t>
+  </si>
+  <si>
+    <t>Nombre y edad de 2 personas y imprimir quien es menor o en todo caso imprimir si tiene la misma edad</t>
+  </si>
+  <si>
+    <t>Leer 5 numeros y obtener el promedio asi como determinar cual es el mas cercano al promedio</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leer un valor y determinar si Es par si el numero N es par, en caso contrario Es impar </t>
+  </si>
+  <si>
+    <t>Realizar la Sucesion de Fibonacci</t>
+  </si>
+  <si>
+    <t>Tengo el promedio solo me falta poner cual es el valor mas sercano al promedio</t>
+  </si>
+  <si>
+    <t>Me falta nostrar los resultados en el HTML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -60,8 +107,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -102,27 +162,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -390,47 +483,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.375" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="4" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -447,16 +545,20 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -473,16 +575,20 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -499,16 +605,20 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -525,16 +635,20 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -551,16 +665,20 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -577,16 +695,20 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -603,16 +725,20 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -629,16 +755,22 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -655,16 +787,20 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -681,16 +817,16 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -707,16 +843,16 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -733,16 +869,16 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -759,16 +895,16 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -785,16 +921,16 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -811,16 +947,14 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -837,16 +971,14 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -863,16 +995,14 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -889,16 +1019,14 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -915,16 +1043,14 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -941,16 +1067,14 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -967,16 +1091,14 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -993,16 +1115,14 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1019,16 +1139,14 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1045,16 +1163,14 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1071,16 +1187,14 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1097,16 +1211,14 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1123,16 +1235,14 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1149,16 +1259,14 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1175,16 +1283,14 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1202,6 +1308,217 @@
       <c r="V31" s="1"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{4278F6C0-0133-4611-A490-3F04B2D80DD1}">
+      <formula1>"En proceso,Con dudas,Terminado"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F084648-7E66-483D-947B-70035FFB7141}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="2" max="2" width="55.25" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="35.25" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C15" xr:uid="{EDC07D19-2ADD-4FD2-8BCE-D101E39E9610}">
+      <formula1>"En proceso,Con dudas,Terminado"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>